<commit_message>
Benchmarks established for preallocated nodes versions of blocking and nonblocking
</commit_message>
<xml_diff>
--- a/Assignments/Assignment2/Benchmarks.xlsx
+++ b/Assignments/Assignment2/Benchmarks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitty/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitty/Documents/COP4934/Assignments/Assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20540" windowHeight="16060"/>
+    <workbookView xWindow="7720" yWindow="1920" windowWidth="20540" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -307,25 +307,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>51910.0</c:v>
+                  <c:v>31453.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26894.0</c:v>
+                  <c:v>17598.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15142.0</c:v>
+                  <c:v>11963.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15106.0</c:v>
+                  <c:v>12228.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14732.0</c:v>
+                  <c:v>11857.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14930.0</c:v>
+                  <c:v>11698.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14892.0</c:v>
+                  <c:v>11465.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,25 +400,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>33161.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36705.0</c:v>
+                  <c:v>663.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36364.0</c:v>
+                  <c:v>739.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36121.0</c:v>
+                  <c:v>765.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36353.0</c:v>
+                  <c:v>745.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36349.0</c:v>
+                  <c:v>749.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36492.0</c:v>
+                  <c:v>776.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,11 +439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1501180080"/>
-        <c:axId val="-1501169344"/>
+        <c:axId val="386145920"/>
+        <c:axId val="367796448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1501180080"/>
+        <c:axId val="386145920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501169344"/>
+        <c:crossAx val="367796448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1501169344"/>
+        <c:axId val="367796448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501180080"/>
+        <c:crossAx val="386145920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -880,25 +880,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>83262.0</c:v>
+                  <c:v>49534.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43065.0</c:v>
+                  <c:v>27404.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23733.0</c:v>
+                  <c:v>17104.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23784.0</c:v>
+                  <c:v>16791.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23481.0</c:v>
+                  <c:v>17610.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24023.0</c:v>
+                  <c:v>16824.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23915.0</c:v>
+                  <c:v>17088.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -973,25 +973,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>54276.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57271.0</c:v>
+                  <c:v>734.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56791.0</c:v>
+                  <c:v>779.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57115.0</c:v>
+                  <c:v>754.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57635.0</c:v>
+                  <c:v>747.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57161.0</c:v>
+                  <c:v>757.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59209.0</c:v>
+                  <c:v>754.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,11 +1012,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1501021360"/>
-        <c:axId val="-1501012688"/>
+        <c:axId val="367836816"/>
+        <c:axId val="367860400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1501021360"/>
+        <c:axId val="367836816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501012688"/>
+        <c:crossAx val="367860400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1501012688"/>
+        <c:axId val="367860400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501021360"/>
+        <c:crossAx val="367836816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1455,10 +1455,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>84593.0</c:v>
+                  <c:v>48540.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43655.0</c:v>
+                  <c:v>26953.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24052.0</c:v>
@@ -1548,10 +1548,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>57281.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57471.0</c:v>
+                  <c:v>679.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>57814.0</c:v>
@@ -1587,11 +1587,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1500288816"/>
-        <c:axId val="-1500280288"/>
+        <c:axId val="386291552"/>
+        <c:axId val="367819744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1500288816"/>
+        <c:axId val="386291552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1500280288"/>
+        <c:crossAx val="367819744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1500280288"/>
+        <c:axId val="367819744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1808,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1500288816"/>
+        <c:crossAx val="386291552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3577,7 +3577,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A412E19D-B20A-41EB-A58B-725CBE836FBA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A412E19D-B20A-41EB-A58B-725CBE836FBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3613,7 +3613,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E6CC3BE-C2A4-4E52-968C-68380AAB30F5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6CC3BE-C2A4-4E52-968C-68380AAB30F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3649,7 +3649,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7352A349-1BFE-44F9-B3C1-B344D36D89CD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7352A349-1BFE-44F9-B3C1-B344D36D89CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3975,7 +3975,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4030,22 +4030,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>51910</v>
+        <v>31453</v>
       </c>
       <c r="C3" s="2">
-        <v>33161</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
-        <v>83262</v>
+        <v>49534</v>
       </c>
       <c r="E3" s="2">
-        <v>54276</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
-        <v>84593</v>
+        <v>48540</v>
       </c>
       <c r="G3" s="2">
-        <v>57281</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4053,22 +4053,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>26894</v>
+        <v>17598</v>
       </c>
       <c r="C4" s="2">
-        <v>36705</v>
+        <v>663</v>
       </c>
       <c r="D4" s="2">
-        <v>43065</v>
+        <v>27404</v>
       </c>
       <c r="E4" s="2">
-        <v>57271</v>
+        <v>734</v>
       </c>
       <c r="F4" s="2">
-        <v>43655</v>
+        <v>26953</v>
       </c>
       <c r="G4" s="2">
-        <v>57471</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4076,16 +4076,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>15142</v>
+        <v>11963</v>
       </c>
       <c r="C5" s="2">
-        <v>36364</v>
+        <v>739</v>
       </c>
       <c r="D5" s="2">
-        <v>23733</v>
+        <v>17104</v>
       </c>
       <c r="E5" s="2">
-        <v>56791</v>
+        <v>779</v>
       </c>
       <c r="F5" s="2">
         <v>24052</v>
@@ -4099,16 +4099,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>15106</v>
+        <v>12228</v>
       </c>
       <c r="C6" s="2">
-        <v>36121</v>
+        <v>765</v>
       </c>
       <c r="D6" s="2">
-        <v>23784</v>
+        <v>16791</v>
       </c>
       <c r="E6" s="2">
-        <v>57115</v>
+        <v>754</v>
       </c>
       <c r="F6" s="2">
         <v>23893</v>
@@ -4122,16 +4122,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>14732</v>
+        <v>11857</v>
       </c>
       <c r="C7" s="2">
-        <v>36353</v>
+        <v>745</v>
       </c>
       <c r="D7" s="2">
-        <v>23481</v>
+        <v>17610</v>
       </c>
       <c r="E7" s="2">
-        <v>57635</v>
+        <v>747</v>
       </c>
       <c r="F7" s="2">
         <v>23717</v>
@@ -4145,16 +4145,16 @@
         <v>32</v>
       </c>
       <c r="B8" s="2">
-        <v>14930</v>
+        <v>11698</v>
       </c>
       <c r="C8" s="2">
-        <v>36349</v>
+        <v>749</v>
       </c>
       <c r="D8" s="2">
-        <v>24023</v>
+        <v>16824</v>
       </c>
       <c r="E8" s="2">
-        <v>57161</v>
+        <v>757</v>
       </c>
       <c r="F8" s="2">
         <v>23794</v>
@@ -4168,16 +4168,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2">
-        <v>14892</v>
+        <v>11465</v>
       </c>
       <c r="C9" s="2">
-        <v>36492</v>
+        <v>776</v>
       </c>
       <c r="D9" s="2">
-        <v>23915</v>
+        <v>17088</v>
       </c>
       <c r="E9" s="2">
-        <v>59209</v>
+        <v>754</v>
       </c>
       <c r="F9" s="2">
         <v>23706</v>

</xml_diff>

<commit_message>
Change probability assignment approach and rerun benchmark tests
</commit_message>
<xml_diff>
--- a/Assignments/Assignment2/Benchmarks.xlsx
+++ b/Assignments/Assignment2/Benchmarks.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27309"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitty/Documents/COP4934/Assignments/Assignment2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lara/COP4934/Assignments/Assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="1920" windowWidth="20540" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,19 +47,19 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Test 3</t>
-  </si>
-  <si>
     <t>Test 1 (mixed)</t>
   </si>
   <si>
     <t>Test 2 (write-dominated)</t>
   </si>
   <si>
-    <t>Computed using 2.9GHz quad-core Intel i5 (4 cores, 4 logical processors)</t>
+    <t xml:space="preserve">200000 operations evenly divided between threads. </t>
   </si>
   <si>
-    <t xml:space="preserve">200000 operations evenly divided between threads. </t>
+    <t>Computed using 3.1 GHz Intel Core i7 quad-core processor (4 physical, 8 logical)</t>
+  </si>
+  <si>
+    <t>Test 3 (read-dominated)</t>
   </si>
 </sst>
 </file>
@@ -307,25 +307,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>31453.0</c:v>
+                  <c:v>48193.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17598.0</c:v>
+                  <c:v>24859.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11963.0</c:v>
+                  <c:v>13616.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12228.0</c:v>
+                  <c:v>8894.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11857.0</c:v>
+                  <c:v>8809.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11698.0</c:v>
+                  <c:v>8627.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11465.0</c:v>
+                  <c:v>8830.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,25 +400,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.0</c:v>
+                  <c:v>31500.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>663.0</c:v>
+                  <c:v>33891.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>739.0</c:v>
+                  <c:v>33402.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>765.0</c:v>
+                  <c:v>33360.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>745.0</c:v>
+                  <c:v>34403.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>749.0</c:v>
+                  <c:v>34103.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>776.0</c:v>
+                  <c:v>34062.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,11 +439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="386145920"/>
-        <c:axId val="367796448"/>
+        <c:axId val="-2097580080"/>
+        <c:axId val="-2097572128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="386145920"/>
+        <c:axId val="-2097580080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367796448"/>
+        <c:crossAx val="-2097572128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="367796448"/>
+        <c:axId val="-2097572128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386145920"/>
+        <c:crossAx val="-2097580080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -880,25 +880,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>49534.0</c:v>
+                  <c:v>77836.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27404.0</c:v>
+                  <c:v>40038.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17104.0</c:v>
+                  <c:v>21839.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16791.0</c:v>
+                  <c:v>13515.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17610.0</c:v>
+                  <c:v>13439.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16824.0</c:v>
+                  <c:v>13227.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17088.0</c:v>
+                  <c:v>13200.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -973,25 +973,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.0</c:v>
+                  <c:v>49608.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>734.0</c:v>
+                  <c:v>53456.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>779.0</c:v>
+                  <c:v>53193.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>754.0</c:v>
+                  <c:v>53357.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>747.0</c:v>
+                  <c:v>53284.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>757.0</c:v>
+                  <c:v>53641.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>754.0</c:v>
+                  <c:v>53659.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,11 +1012,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="367836816"/>
-        <c:axId val="367860400"/>
+        <c:axId val="-2097493120"/>
+        <c:axId val="-2097487056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="367836816"/>
+        <c:axId val="-2097493120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367860400"/>
+        <c:crossAx val="-2097487056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="367860400"/>
+        <c:axId val="-2097487056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367836816"/>
+        <c:crossAx val="-2097493120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1455,25 +1455,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>48540.0</c:v>
+                  <c:v>18089.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26953.0</c:v>
+                  <c:v>9499.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24052.0</c:v>
+                  <c:v>5229.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23893.0</c:v>
+                  <c:v>3931.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23717.0</c:v>
+                  <c:v>3881.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23794.0</c:v>
+                  <c:v>4001.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23706.0</c:v>
+                  <c:v>3956.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1548,25 +1548,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>11.0</c:v>
+                  <c:v>10130.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>679.0</c:v>
+                  <c:v>12097.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57814.0</c:v>
+                  <c:v>11814.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58630.0</c:v>
+                  <c:v>11978.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59230.0</c:v>
+                  <c:v>12494.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61837.0</c:v>
+                  <c:v>12622.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61390.0</c:v>
+                  <c:v>12714.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,11 +1587,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="386291552"/>
-        <c:axId val="367819744"/>
+        <c:axId val="-2097445984"/>
+        <c:axId val="-2097439920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="386291552"/>
+        <c:axId val="-2097445984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367819744"/>
+        <c:crossAx val="-2097439920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="367819744"/>
+        <c:axId val="-2097439920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1808,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386291552"/>
+        <c:crossAx val="-2097445984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3577,7 +3577,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A412E19D-B20A-41EB-A58B-725CBE836FBA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A412E19D-B20A-41EB-A58B-725CBE836FBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3613,7 +3613,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6CC3BE-C2A4-4E52-968C-68380AAB30F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E6CC3BE-C2A4-4E52-968C-68380AAB30F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3649,7 +3649,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7352A349-1BFE-44F9-B3C1-B344D36D89CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7352A349-1BFE-44F9-B3C1-B344D36D89CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3975,7 +3975,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3992,15 +3992,15 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G1" s="4"/>
     </row>
@@ -4030,22 +4030,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>31453</v>
+        <v>48193</v>
       </c>
       <c r="C3" s="2">
-        <v>12</v>
+        <v>31500</v>
       </c>
       <c r="D3" s="2">
-        <v>49534</v>
+        <v>77836</v>
       </c>
       <c r="E3" s="2">
-        <v>12</v>
+        <v>49608</v>
       </c>
       <c r="F3" s="2">
-        <v>48540</v>
+        <v>18089</v>
       </c>
       <c r="G3" s="2">
-        <v>11</v>
+        <v>10130</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4053,22 +4053,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>17598</v>
+        <v>24859</v>
       </c>
       <c r="C4" s="2">
-        <v>663</v>
+        <v>33891</v>
       </c>
       <c r="D4" s="2">
-        <v>27404</v>
+        <v>40038</v>
       </c>
       <c r="E4" s="2">
-        <v>734</v>
+        <v>53456</v>
       </c>
       <c r="F4" s="2">
-        <v>26953</v>
+        <v>9499</v>
       </c>
       <c r="G4" s="2">
-        <v>679</v>
+        <v>12097</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4076,22 +4076,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>11963</v>
+        <v>13616</v>
       </c>
       <c r="C5" s="2">
-        <v>739</v>
+        <v>33402</v>
       </c>
       <c r="D5" s="2">
-        <v>17104</v>
+        <v>21839</v>
       </c>
       <c r="E5" s="2">
-        <v>779</v>
+        <v>53193</v>
       </c>
       <c r="F5" s="2">
-        <v>24052</v>
+        <v>5229</v>
       </c>
       <c r="G5" s="2">
-        <v>57814</v>
+        <v>11814</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4099,22 +4099,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>12228</v>
+        <v>8894</v>
       </c>
       <c r="C6" s="2">
-        <v>765</v>
+        <v>33360</v>
       </c>
       <c r="D6" s="2">
-        <v>16791</v>
+        <v>13515</v>
       </c>
       <c r="E6" s="2">
-        <v>754</v>
+        <v>53357</v>
       </c>
       <c r="F6" s="2">
-        <v>23893</v>
+        <v>3931</v>
       </c>
       <c r="G6" s="2">
-        <v>58630</v>
+        <v>11978</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4122,22 +4122,22 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>11857</v>
+        <v>8809</v>
       </c>
       <c r="C7" s="2">
-        <v>745</v>
+        <v>34403</v>
       </c>
       <c r="D7" s="2">
-        <v>17610</v>
+        <v>13439</v>
       </c>
       <c r="E7" s="2">
-        <v>747</v>
+        <v>53284</v>
       </c>
       <c r="F7" s="2">
-        <v>23717</v>
+        <v>3881</v>
       </c>
       <c r="G7" s="2">
-        <v>59230</v>
+        <v>12494</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -4145,22 +4145,22 @@
         <v>32</v>
       </c>
       <c r="B8" s="2">
-        <v>11698</v>
+        <v>8627</v>
       </c>
       <c r="C8" s="2">
-        <v>749</v>
+        <v>34103</v>
       </c>
       <c r="D8" s="2">
-        <v>16824</v>
+        <v>13227</v>
       </c>
       <c r="E8" s="2">
-        <v>757</v>
+        <v>53641</v>
       </c>
       <c r="F8" s="2">
-        <v>23794</v>
+        <v>4001</v>
       </c>
       <c r="G8" s="2">
-        <v>61837</v>
+        <v>12622</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4168,22 +4168,22 @@
         <v>64</v>
       </c>
       <c r="B9" s="2">
-        <v>11465</v>
+        <v>8830</v>
       </c>
       <c r="C9" s="2">
-        <v>776</v>
+        <v>34062</v>
       </c>
       <c r="D9" s="2">
-        <v>17088</v>
+        <v>13200</v>
       </c>
       <c r="E9" s="2">
-        <v>754</v>
+        <v>53659</v>
       </c>
       <c r="F9" s="2">
-        <v>23706</v>
+        <v>3956</v>
       </c>
       <c r="G9" s="2">
-        <v>61390</v>
+        <v>12714</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4191,7 +4191,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix pre-allocation bug, rerun benchmarks, modify probability assignment approach
</commit_message>
<xml_diff>
--- a/Assignments/Assignment2/Benchmarks.xlsx
+++ b/Assignments/Assignment2/Benchmarks.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lara/COP4934/Assignments/Assignment2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitty/Documents/COP4934/Assignments/Assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,10 @@
     <t xml:space="preserve">200000 operations evenly divided between threads. </t>
   </si>
   <si>
-    <t>Computed using 3.1 GHz Intel Core i7 quad-core processor (4 physical, 8 logical)</t>
+    <t>Test 3 (read-dominated)</t>
   </si>
   <si>
-    <t>Test 3 (read-dominated)</t>
+    <t xml:space="preserve">Computed using 3.1 GHz Intel Core i7 quad-core processor (4 physical, 8 logical) </t>
   </si>
 </sst>
 </file>
@@ -439,11 +439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2097580080"/>
-        <c:axId val="-2097572128"/>
+        <c:axId val="1140792688"/>
+        <c:axId val="1140801344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2097580080"/>
+        <c:axId val="1140792688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097572128"/>
+        <c:crossAx val="1140801344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097572128"/>
+        <c:axId val="1140801344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097580080"/>
+        <c:crossAx val="1140792688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1012,11 +1012,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2097493120"/>
-        <c:axId val="-2097487056"/>
+        <c:axId val="1140662448"/>
+        <c:axId val="1140648688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2097493120"/>
+        <c:axId val="1140662448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097487056"/>
+        <c:crossAx val="1140648688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097487056"/>
+        <c:axId val="1140648688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097493120"/>
+        <c:crossAx val="1140662448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1587,11 +1587,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2097445984"/>
-        <c:axId val="-2097439920"/>
+        <c:axId val="1179747824"/>
+        <c:axId val="1179751216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2097445984"/>
+        <c:axId val="1179747824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097439920"/>
+        <c:crossAx val="1179751216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097439920"/>
+        <c:axId val="1179751216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1808,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097445984"/>
+        <c:crossAx val="1179747824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3975,7 +3975,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4000,7 +4000,7 @@
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
     </row>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>